<commit_message>
added support for newer version of xlrd
</commit_message>
<xml_diff>
--- a/Crypto.xlsx
+++ b/Crypto.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2571385</v>
+        <v>2416933</v>
       </c>
       <c r="C2" t="n">
         <v>0.001</v>
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>109096.4</v>
+        <v>100400</v>
       </c>
       <c r="C3" t="n">
         <v>0.003</v>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21.2512</v>
+        <v>19.9</v>
       </c>
       <c r="C4" t="n">
         <v>0.01</v>
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.4098</v>
+        <v>2.255</v>
       </c>
       <c r="C5" t="n">
         <v>0.22</v>

</xml_diff>

<commit_message>
fixed null index error
</commit_message>
<xml_diff>
--- a/Crypto.xlsx
+++ b/Crypto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,61 +446,96 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Holdings</t>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Volume</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Profit/Loss</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>P/L%</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>btcinr</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2416933</v>
+        <v>2765392</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001</v>
-      </c>
+        <v>2199000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>ethinr</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>100400</v>
+        <v>120206.6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003</v>
-      </c>
+        <v>120000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>xrpinr</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19.9</v>
+        <v>29.5183</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>123</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>trxinr</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.255</v>
+        <v>2.4697</v>
       </c>
       <c r="C5" t="n">
-        <v>0.22</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2334</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>